<commit_message>
Adecuacion de la implementacion de lectura excel para credito empresarial
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarial.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t xml:space="preserve"> Monto</t>
   </si>
@@ -114,6 +114,27 @@
   </si>
   <si>
     <t>LIMA</t>
+  </si>
+  <si>
+    <t>S/</t>
+  </si>
+  <si>
+    <t>Moneda</t>
+  </si>
+  <si>
+    <t>2363</t>
+  </si>
+  <si>
+    <t>2517</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Comentarios Ratios</t>
   </si>
 </sst>
 </file>
@@ -156,9 +177,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -441,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -455,18 +480,20 @@
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="19.42578125" customWidth="1"/>
-    <col min="17" max="17" width="30" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="19.42578125" customWidth="1"/>
+    <col min="18" max="18" width="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30" customWidth="1"/>
+    <col min="20" max="20" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -486,48 +513,54 @@
         <v>21</v>
       </c>
       <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>26</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>27</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
-      <c r="A2">
-        <v>2363</v>
+    <row r="2" spans="1:21">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
@@ -544,29 +577,29 @@
       <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2">
         <v>1000</v>
       </c>
-      <c r="H2">
+      <c r="I2" s="2">
         <v>1</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="1">
-        <v>90</v>
-      </c>
-      <c r="L2" s="1">
-        <v>30</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="L2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>29</v>
@@ -574,19 +607,25 @@
       <c r="P2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" t="s">
         <v>15</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
-      <c r="A3">
-        <v>2517</v>
+    <row r="3" spans="1:21">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
@@ -603,29 +642,29 @@
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2">
         <v>4500</v>
       </c>
-      <c r="H3">
+      <c r="I3" s="2">
         <v>2</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="1">
-        <v>90</v>
-      </c>
-      <c r="L3" s="1">
-        <v>30</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="L3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>29</v>
@@ -633,13 +672,19 @@
       <c r="P3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" t="s">
         <v>15</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios en lectura de excel de credito Empresarial
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarial.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t xml:space="preserve"> Monto</t>
   </si>
@@ -122,19 +122,34 @@
     <t>Moneda</t>
   </si>
   <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Comentarios Ratios</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
     <t>2363</t>
   </si>
   <si>
-    <t>2517</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>Comentarios Ratios</t>
+    <t>Numero Propuesta</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>2240</t>
   </si>
 </sst>
 </file>
@@ -466,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -493,7 +508,7 @@
     <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -549,7 +564,7 @@
         <v>16</v>
       </c>
       <c r="S1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="T1" t="s">
         <v>12</v>
@@ -557,10 +572,16 @@
       <c r="U1" t="s">
         <v>11</v>
       </c>
+      <c r="V1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:23">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
@@ -580,11 +601,11 @@
       <c r="G2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1</v>
+      <c r="H2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>14</v>
@@ -593,10 +614,10 @@
         <v>23</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>25</v>
@@ -622,10 +643,13 @@
       <c r="U2" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="W2" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:23">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
@@ -645,11 +669,11 @@
       <c r="G3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="2">
-        <v>4500</v>
-      </c>
-      <c r="I3" s="2">
-        <v>2</v>
+      <c r="H3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>14</v>
@@ -658,10 +682,10 @@
         <v>23</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>25</v>
@@ -686,6 +710,9 @@
       </c>
       <c r="U3" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="W3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios de escritura excel
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarial.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CajaPiuraCMAC2021\target\DatosExcel\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t xml:space="preserve"> Monto</t>
   </si>
@@ -137,25 +137,20 @@
     <t>5000</t>
   </si>
   <si>
-    <t>2363</t>
-  </si>
-  <si>
-    <t>Numero Propuesta</t>
-  </si>
-  <si>
-    <t>Resultado</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
     <t>2240</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -481,34 +476,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="19.42578125" customWidth="1"/>
-    <col min="18" max="18" width="30" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="30" customWidth="1"/>
-    <col min="20" max="20" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.0" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="18.140625" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="9.5703125" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="13.85546875" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="9.28515625" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="20.5703125" collapsed="false"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="15" max="17" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="30.0" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" width="30.0" collapsed="false"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="28.85546875" collapsed="false"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -575,11 +570,8 @@
       <c r="V1" t="s">
         <v>38</v>
       </c>
-      <c r="W1" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:21">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -643,76 +635,8 @@
       <c r="U2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23">
-      <c r="A3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T3" t="s">
-        <v>17</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="W3" t="s">
-        <v>40</v>
+      <c r="V2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Cambios de escritura excel"
This reverts commit dc24a201ab87cde3b57652189d413b2c654af520.
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarial.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CajaPiuraCMAC2021\target\DatosExcel\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t xml:space="preserve"> Monto</t>
   </si>
@@ -137,20 +137,25 @@
     <t>5000</t>
   </si>
   <si>
+    <t>2363</t>
+  </si>
+  <si>
+    <t>Numero Propuesta</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
     <t>2240</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -476,34 +481,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.0" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="18.140625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="9.5703125" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="13.85546875" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="19.42578125" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="9.28515625" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="20.5703125" collapsed="false"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
-    <col min="15" max="17" customWidth="true" width="19.42578125" collapsed="false"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="30.0" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" width="30.0" collapsed="false"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="28.85546875" collapsed="false"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="19.42578125" customWidth="1"/>
+    <col min="18" max="18" width="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30" customWidth="1"/>
+    <col min="20" max="20" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -570,8 +575,11 @@
       <c r="V1" t="s">
         <v>38</v>
       </c>
+      <c r="W1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:23">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -635,8 +643,76 @@
       <c r="U2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V2" t="s">
-        <v>39</v>
+      <c r="W2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios realizados antes de iniciar con entregable diciembre
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarial.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Cliente</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Comentarios Ratios</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Servicio Credito </t>
   </si>
   <si>
@@ -134,25 +131,31 @@
     <t>Monto</t>
   </si>
   <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>1331906</t>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>Numero Propuesta</t>
+  </si>
+  <si>
+    <t>Tipo Operación</t>
+  </si>
+  <si>
+    <t>SIMPLE</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
   <si>
     <t>2000</t>
   </si>
   <si>
-    <t>1332236</t>
-  </si>
-  <si>
-    <t>Resultado</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
+    <t>1343556</t>
+  </si>
+  <si>
+    <t>4899845</t>
+  </si>
+  <si>
+    <t>El Documento ha sido derivado satisfactoriamente</t>
   </si>
 </sst>
 </file>
@@ -176,7 +179,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +189,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -202,12 +211,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9:U10"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -501,133 +513,140 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="15" max="17" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="16" max="18" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="48.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" t="s">
+    <row r="1" spans="1:24">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
       </c>
       <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V1" t="s">
+    </row>
+    <row r="2" spans="1:24" s="4" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>25</v>
@@ -636,89 +655,29 @@
         <v>25</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="T2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="V2" t="s">
-        <v>41</v>
+      <c r="W2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V3" t="s">
-        <v>42</v>
-      </c>
-    </row>
+    <row r="3" spans="1:24" s="4" customFormat="1"/>
+    <row r="4" spans="1:24" s="4" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
agregar tiempo a la ventana checklist
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarial.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CajaPiuraCMAC2021\target\DatosExcel\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -152,17 +152,16 @@
     <t>1343556</t>
   </si>
   <si>
-    <t>4899845</t>
-  </si>
-  <si>
     <t>El Documento ha sido derivado satisfactoriamente</t>
+  </si>
+  <si>
+    <t>4900028</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -502,30 +501,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2:X2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="16" max="18" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="48.5703125" collapsed="true"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.28515625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="18" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="30" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="48.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -670,10 +667,10 @@
         <v>14</v>
       </c>
       <c r="W2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" t="s">
         <v>42</v>
-      </c>
-      <c r="X2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="4" customFormat="1"/>

</xml_diff>